<commit_message>
Code Home Template, Add Layouts, Add Modules, AddTemplates
</commit_message>
<xml_diff>
--- a/Công việc/CV.xlsx
+++ b/Công việc/CV.xlsx
@@ -1,26 +1,582 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\Dự án tốt nghiệp\TMDT\Công việc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01593475-41D7-48BF-888A-F91467249004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Tên công việc</t>
+  </si>
+  <si>
+    <t>Mô tả</t>
+  </si>
+  <si>
+    <t>Code giao diện</t>
+  </si>
+  <si>
+    <t>Thời gian thực hiện</t>
+  </si>
+  <si>
+    <t>Code template HOME</t>
+  </si>
+  <si>
+    <t>&lt;!DOCTYPE html&gt;_x000D_
+&lt;html lang="en"&gt;_x000D_
+_x000D_
+&lt;head&gt;_x000D_
+    _x000D_
+    &lt;meta charset="utf-8"&gt;_x000D_
+    &lt;meta name="viewport" content="width=device-width, initial-scale=1.0, user-scalable=no"&gt;_x000D_
+    &lt;meta name="description" content=""&gt;_x000D_
+    &lt;meta name="author" content=""&gt;_x000D_
+    &lt;meta name="keywords" content=""&gt;_x000D_
+    &lt;meta name="robots" content="all"&gt;_x000D_
+    &lt;title&gt;@yield('title')&lt;/title&gt;_x000D_
+_x000D_
+    _x000D_
+    &lt;link rel="stylesheet" href="{{ asset('client/assets/css/bootstrap.min.css') }}"&gt;_x000D_
+_x000D_
+    _x000D_
+    &lt;link rel="stylesheet" href="{{ asset('client/assets/css/main.css') }}"&gt;_x000D_
+    &lt;link rel="stylesheet" href="{{ asset('client/assets/css/blue.css') }}"&gt;_x000D_
+    &lt;link rel="stylesheet" href="{{ asset('client/assets/css/owl.carousel.css') }}"&gt;_x000D_
+    &lt;link rel="stylesheet" href="{{ asset('client/assets/css/owl.transitions.css') }}"&gt;_x000D_
+    &lt;link rel="stylesheet" href="{{ asset('client/assets/css/animate.min.css') }}"&gt;_x000D_
+    &lt;link rel="stylesheet" href="{{ asset('client/assets/css/rateit.css') }}"&gt;_x000D_
+    &lt;link rel="stylesheet" href="{{ asset('client/assets/css/bootstrap-select.min.css') }}"&gt;_x000D_
+    &lt;link rel="stylesheet" href="{{ asset('client/assets/css/do.css') }}"&gt;_x000D_
+_x000D_
+    _x000D_
+    &lt;link rel="stylesheet" href="{{ asset('client/assets/css/font-awesome.css') }}"&gt;_x000D_
+_x000D_
+    &lt;link rel="stylesheet" href="https://cdnjs.cloudflare.com/ajax/libs/font-awesome/6.4.0/css/all.min.css" /&gt;_x000D_
+_x000D_
+    _x000D_
+    &lt;link href='http://fonts.googleapis.com/css?family=Roboto:300,400,500,700' rel='stylesheet' type='text/css'&gt;_x000D_
+    &lt;link href='https://fonts.googleapis.com/css?family=Open+Sans:400,300,400italic,600,600italic,700,700italic,800'_x000D_
+        rel='stylesheet' type='text/css'&gt;_x000D_
+    &lt;link href='https://fonts.googleapis.com/css?family=Montserrat:400,700' rel='stylesheet' type='text/css'&gt;_x000D_
+&lt;/head&gt;_x000D_
+_x000D_
+&lt;body class="cnt-home"&gt;_x000D_
+    _x000D_
+    &lt;header class="header-style-1"&gt;_x000D_
+        _x000D_
+        &lt;div class="top-bar animate-dropdown"&gt;_x000D_
+            &lt;div class="container"&gt;_x000D_
+                &lt;div class="header-top-inner"&gt;_x000D_
+                    &lt;div class="cnt-account"&gt;_x000D_
+                        &lt;ul class="list-unstyled"&gt;_x000D_
+                            &lt;li&gt;&lt;a href="#"&gt;&lt;i class="fa fa-download"&gt;&lt;/i&gt; Táº£i app&lt;/a&gt;&lt;/li&gt;_x000D_
+                            &lt;li&gt;&lt;a href="#"&gt;&lt;i class="fas fa-map-marker-alt"&gt;&lt;/i&gt; Há»‡ thá»‘ng 50 cá»­a hĂ ng&lt;/a&gt;&lt;/li&gt;_x000D_
+                            &lt;li&gt;&lt;a href="#"&gt;&lt;i class="fa fa-envelope-open-o"&gt;&lt;/i&gt; ChĂ­nh sĂ¡ch báº£o hĂ nh &amp; Ä‘á»•i_x000D_
+                                    tráº£&lt;/a&gt;&lt;/li&gt;_x000D_
+                            &lt;li&gt;&lt;a href="#"&gt;&lt;i class="fa fa-comment"&gt;&lt;/i&gt; GĂ³p Ă½ &amp; pháº£n há»“i&lt;/a&gt;&lt;/li&gt;_x000D_
+                            &lt;li&gt;&lt;a href="#"&gt;&lt;i class="fas fa-box"&gt;&lt;/i&gt; Theo dĂµi Ä‘Æ¡n hĂ ng&lt;/a&gt;&lt;/li&gt;_x000D_
+                            &lt;li&gt;&lt;a href="#"&gt;&lt;i class="icon fa fa-user"&gt;&lt;/i&gt; ÄÄƒng kĂ½/ÄÄƒng nháº­p&lt;/a&gt;&lt;/li&gt;_x000D_
+                        &lt;/ul&gt;_x000D_
+                    &lt;/div&gt;_x000D_
+                    _x000D_
+_x000D_
+                    &lt;div class="cnt-block"&gt;_x000D_
+                        &lt;ul class="list-unstyled list-inline"&gt;_x000D_
+                            &lt;li class="dropdown dropdown-small"&gt; &lt;a href="#" class="dropdown-toggle"_x000D_
+                                    data-hover="dropdown" data-toggle="dropdown"&gt;&lt;span class="value"&gt;VietNamese_x000D_
+                                    &lt;/span&gt;&lt;b class="caret"&gt;&lt;/b&gt;&lt;/a&gt;_x000D_
+                                &lt;ul class="dropdown-menu"&gt;_x000D_
+                                    &lt;li&gt;&lt;a href="#"&gt;VietNamese&lt;/a&gt;&lt;/li&gt;_x000D_
+                                    &lt;li&gt;&lt;a href="#"&gt;French&lt;/a&gt;&lt;/li&gt;_x000D_
+                                    &lt;li&gt;&lt;a href="#"&gt;English&lt;/a&gt;&lt;/li&gt;_x000D_
+                                &lt;/ul&gt;_x000D_
+                            &lt;/li&gt;_x000D_
+                        &lt;/ul&gt;_x000D_
+                        _x000D_
+                    &lt;/div&gt;_x000D_
+                    _x000D_
+                    &lt;div class="clearfix"&gt;&lt;/div&gt;_x000D_
+                &lt;/div&gt;_x000D_
+                _x000D_
+            &lt;/div&gt;_x000D_
+            _x000D_
+        &lt;/div&gt;_x000D_
+        _x000D_
+        _x000D_
+        &lt;div class="main-header"&gt;_x000D_
+            &lt;div class="container"&gt;_x000D_
+                &lt;div class="row"&gt;_x000D_
+                    &lt;div class="col-xs-12 col-sm-12 col-md-3 logo-holder"&gt;_x000D_
+                        _x000D_
+                        &lt;div class="logo"&gt; &lt;a href="home.html"&gt; &lt;img src="assets/images/logo_fnn.png" alt="logo"&gt;_x000D_
+                            &lt;/a&gt; &lt;/div&gt;_x000D_
+                        _x000D_
+                        _x000D_
+                    &lt;/div&gt;_x000D_
+                    _x000D_
+_x000D_
+                    &lt;div class="col-xs-12 col-sm-12 col-md-5 top-search-holder"&gt;_x000D_
+                        _x000D_
+                        _x000D_
+                        &lt;div class="search-area"&gt;_x000D_
+                            &lt;form&gt;_x000D_
+                                &lt;div class="control-group"&gt;_x000D_
+                                    &lt;input class="search-field" placeholder="Báº¡n cáº§n tĂ¬m gĂ¬..."&gt;_x000D_
+                                    &lt;a class="search-button" href="#"&gt;&lt;/a&gt;_x000D_
+                                &lt;/div&gt;_x000D_
+                            &lt;/form&gt;_x000D_
+                        &lt;/div&gt;_x000D_
+                        _x000D_
+                        _x000D_
+                    &lt;/div&gt;_x000D_
+                    _x000D_
+_x000D_
+                    &lt;div class="col-xs-12 col-sm-12 col-md-1 animate-dropdown top-cart-row"&gt;_x000D_
+                        _x000D_
+_x000D_
+                        &lt;div class="dropdown dropdown-cart"&gt; &lt;a href="#" class="dropdown-toggle lnk-cart"_x000D_
+                                data-toggle="dropdown"&gt;_x000D_
+                                &lt;div class="items-cart-inner"&gt;_x000D_
+                                    &lt;div class="basket"&gt;&lt;i class="fas fa-shopping-cart"_x000D_
+                                            style="font-size:26px;color:white"&gt;&lt;/i&gt;&lt;/div&gt;_x000D_
+                                    &lt;div class="basket-item-count"&gt;&lt;span class="count"&gt;1&lt;/span&gt;&lt;/div&gt;_x000D_
+                                &lt;/div&gt;_x000D_
+                            &lt;/a&gt;_x000D_
+                            &lt;ul class="dropdown-menu"&gt;_x000D_
+                                &lt;li&gt;_x000D_
+                                    &lt;div class="cart-item product-summary"&gt;_x000D_
+                                        &lt;div class="row"&gt;_x000D_
+                                            &lt;div class="col-xs-4"&gt;_x000D_
+                                                &lt;div class="image"&gt; &lt;a href="detail.html"&gt;&lt;img_x000D_
+                                                            src="assets\images\cart.jpg" alt=""&gt;&lt;/a&gt; &lt;/div&gt;_x000D_
+                                            &lt;/div&gt;_x000D_
+                                            &lt;div class="col-xs-7"&gt;_x000D_
+                                                &lt;h3 class="name"&gt;&lt;a href="index.php?page-detail"&gt;Simple Product&lt;/a&gt;_x000D_
+                                                &lt;/h3&gt;_x000D_
+                                                &lt;div class="price"&gt;$600.00&lt;/div&gt;_x000D_
+                                            &lt;/div&gt;_x000D_
+                                            &lt;div class="col-xs-1 action"&gt; &lt;a href="#"&gt;&lt;i_x000D_
+                                                        class="fa fa-trash"&gt;&lt;/i&gt;&lt;/a&gt; &lt;/div&gt;_x000D_
+                                        &lt;/div&gt;_x000D_
+                                    &lt;/div&gt;_x000D_
+                                    _x000D_
+                                    &lt;div class="clearfix"&gt;&lt;/div&gt;_x000D_
+                                    &lt;hr&gt;_x000D_
+                                    &lt;div class="clearfix cart-total"&gt;_x000D_
+                                        &lt;div class="pull-right"&gt; &lt;span class="text"&gt;Sub Total :&lt;/span&gt;&lt;span_x000D_
+                                                class='price'&gt;$600.00&lt;/span&gt; &lt;/div&gt;_x000D_
+                                        &lt;div class="clearfix"&gt;&lt;/div&gt;_x000D_
+                                        &lt;a href="checkout.html"_x000D_
+                                            class="btn btn-upper btn-primary btn-block m-t-20"&gt;Checkout&lt;/a&gt;_x000D_
+                                    &lt;/div&gt;_x000D_
+                                    _x000D_
+_x000D_
+                                &lt;/li&gt;_x000D_
+                            &lt;/ul&gt;_x000D_
+                            _x000D_
+                        &lt;/div&gt;_x000D_
+                        _x000D_
+_x000D_
+                        _x000D_
+                    &lt;/div&gt;_x000D_
+                    &lt;div class="col-xs-12 col-sm-12 col-md-2 complain"&gt;_x000D_
+                        _x000D_
+                        &lt;div class="complain"&gt;_x000D_
+                            &lt;a href="home.html"&gt;&lt;i class='fas fa-comments'_x000D_
+                                    style='font-size:30px;color:white'&gt;&lt;/i&gt;&lt;/a&gt;_x000D_
+                            &lt;div class="content-complain"&gt;_x000D_
+                                &lt;span class="text-complain"&gt;Khiáº¿u náº¡i&lt;/br&gt;&lt;/span&gt;_x000D_
+                                &lt;span class="phone-complain"&gt;0123456789&lt;/span&gt;_x000D_
+                            &lt;/div&gt;_x000D_
+                        &lt;/div&gt;_x000D_
+                        _x000D_
+                        _x000D_
+                    &lt;/div&gt;_x000D_
+                    &lt;div class="col-xs-12 col-sm-12 col-md-2 hotline"&gt;_x000D_
+                        _x000D_
+                        &lt;div class="hotline"&gt;_x000D_
+                            &lt;a href="home.html"&gt;&lt;i class="fas fa-phone-alt"_x000D_
+                                    style="font-size:30px;color:white"&gt;&lt;/i&gt;&lt;/a&gt;_x000D_
+                            &lt;div class="content-hotline"&gt;_x000D_
+                                &lt;span class="text-hotline"&gt;Hotline bĂ¡n hĂ ng&lt;/br&gt;&lt;/span&gt;_x000D_
+                                &lt;span class="phone-hotline"&gt;0909 2323&lt;/span&gt;_x000D_
+                            &lt;/div&gt;_x000D_
+                        &lt;/div&gt;_x000D_
+                        _x000D_
+                        _x000D_
+                    &lt;/div&gt;_x000D_
+                    &lt;div class="col-xs-12 col-sm-12 col-md-1 technology"&gt;_x000D_
+                        _x000D_
+                        &lt;div class="technology"&gt;_x000D_
+                            &lt;a href="home.html"&gt;&lt;i class="fas fa-headset" style="font-size:30px;color:white"&gt;&lt;/i&gt;&lt;/a&gt;_x000D_
+                            &lt;div class="content-technology"&gt;_x000D_
+                                &lt;span class="text-technology"&gt;TÆ° váº¥n ká»¹ thuáº­t&lt;/br&gt;&lt;/span&gt;_x000D_
+                                &lt;span class="phone-technology"&gt;0909 1214&lt;/span&gt;_x000D_
+                            &lt;/div&gt;_x000D_
+                        &lt;/div&gt;_x000D_
+                        _x000D_
+                        _x000D_
+                    &lt;/div&gt;_x000D_
+                    _x000D_
+                &lt;/div&gt;_x000D_
+                _x000D_
+_x000D_
+            &lt;/div&gt;_x000D_
+            _x000D_
+_x000D_
+        &lt;/div&gt;_x000D_
+        _x000D_
+_x000D_
+        _x000D_
+        &lt;div class="header-nav animate-dropdown"&gt;_x000D_
+            &lt;div class="container"&gt;_x000D_
+                &lt;div class="yamm navbar navbar-default" role="navigation"&gt;_x000D_
+                    &lt;div class="navbar-header"&gt;_x000D_
+                        &lt;button data-target="#mc-horizontal-menu-collapse" data-toggle="collapse"_x000D_
+                            class="navbar-toggle collapsed" type="button"&gt;_x000D_
+                            &lt;span class="sr-only"&gt;Toggle navigation&lt;/span&gt; &lt;span class="icon-bar"&gt;&lt;/span&gt; &lt;span_x000D_
+                                class="icon-bar"&gt;&lt;/span&gt; &lt;span class="icon-bar"&gt;&lt;/span&gt; &lt;/button&gt;_x000D_
+                    &lt;/div&gt;_x000D_
+                    &lt;div class="nav-bg-class"&gt;_x000D_
+                        &lt;div class="navbar-collapse collapse" id="mc-horizontal-menu-collapse"&gt;_x000D_
+                            &lt;div class="nav-outer"&gt;_x000D_
+                                &lt;ul class="nav navbar-nav"&gt;_x000D_
+                                    &lt;li class="active dropdown yamm-fw"&gt; &lt;a href="home.html" data-hover="dropdown"_x000D_
+                                            class="dropdown-toggle" data-toggle="dropdown"&gt;Home&lt;/a&gt; &lt;/li&gt;_x000D_
+                                    &lt;li class="dropdown yamm mega-menu"&gt; &lt;a href="home.html" data-hover="dropdown"_x000D_
+                                            class="dropdown-toggle" data-toggle="dropdown"&gt;iPhone&lt;/a&gt;_x000D_
+                                        &lt;ul class="dropdown-menu container"&gt;_x000D_
+                                            &lt;li&gt;_x000D_
+                                                &lt;div class="yamm-content "&gt;_x000D_
+                                                    &lt;div class="row"&gt;_x000D_
+                                                        &lt;div class="col-xs-12 col-sm-6 col-md-2 col-menu"&gt;_x000D_
+                                                            &lt;h2 class="title"&gt;iPhone 14 Series&lt;/h2&gt;_x000D_
+                                                            &lt;ul class="links"&gt;_x000D_
+                                                                &lt;li&gt;&lt;a href="#"&gt;iPhone 14 Pro Max&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                                &lt;li&gt;&lt;a href="#"&gt;iPhone 14 Pro&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                                &lt;li&gt;&lt;a href="#"&gt;iPhone 14 Plus&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                                &lt;li&gt;&lt;a href="#"&gt;iPhone 14&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                            &lt;/ul&gt;_x000D_
+                                                        &lt;/div&gt;_x000D_
+                                                        _x000D_
+_x000D_
+                                                        &lt;div class="col-xs-12 col-sm-6 col-md-2 col-menu"&gt;_x000D_
+                                                            &lt;h2 class="title"&gt;iPhone 13 Series&lt;/h2&gt;_x000D_
+                                                            &lt;ul class="links"&gt;_x000D_
+                                                                &lt;li&gt;&lt;a href="#"&gt;iPhone 13 Mini&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                                &lt;li&gt;&lt;a href="#"&gt;iPhone 13&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                                &lt;li&gt;&lt;a href="#"&gt;iPhone 13 Pro &lt;/a&gt;&lt;/li&gt;_x000D_
+                                                                &lt;li&gt;&lt;a href="#"&gt;iPhone 13 Pro Max&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                            &lt;/ul&gt;_x000D_
+                                                        &lt;/div&gt;_x000D_
+                                                        _x000D_
+_x000D_
+                                                        &lt;div class="col-xs-12 col-sm-6 col-md-2 col-menu"&gt;_x000D_
+                                                            &lt;h2 class="title"&gt;iPhone 12 Series&lt;/h2&gt;_x000D_
+                                                            &lt;ul class="links"&gt;_x000D_
+                                                                &lt;li&gt;&lt;a href="#"&gt;iPhone 12&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                            &lt;/ul&gt;_x000D_
+                                                        &lt;/div&gt;_x000D_
+                                                        _x000D_
+_x000D_
+                                                        &lt;div class="col-xs-12 col-sm-6 col-md-2 col-menu"&gt;_x000D_
+                                                            &lt;h2 class="title"&gt;iPhone 11 Series&lt;/h2&gt;_x000D_
+                                                            &lt;ul class="links"&gt;_x000D_
+                                                                &lt;li&gt;&lt;a href="#"&gt;iPhone 11&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                                &lt;li&gt;&lt;a href="#"&gt;iPhone 11 Pro&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                                &lt;li&gt;&lt;a href="#"&gt;iPhone 11 Pro Max&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                            &lt;/ul&gt;_x000D_
+                                                        &lt;/div&gt;_x000D_
+                                                        _x000D_
+                                                        &lt;div class="col-xs-12 col-sm-6 col-md-2 col-menu"&gt;_x000D_
+                                                            &lt;h2 class="title"&gt;iPhone XS / iPhone XS Max&lt;/h2&gt;_x000D_
+                                                            &lt;ul class="links"&gt;_x000D_
+                                                                &lt;li&gt;&lt;a href="#"&gt;iPhone XS&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                                &lt;li&gt;&lt;a href="#"&gt;iPhone XS Max&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                            &lt;/ul&gt;_x000D_
+                                                        &lt;/div&gt;_x000D_
+                                                        _x000D_
+                                                        &lt;div class="col-xs-12 col-sm-6 col-md-2 col-menu"&gt;_x000D_
+                                                            &lt;h2 class="title"&gt;iPhone X / iPhone XR&lt;/h2&gt;_x000D_
+                                                            &lt;ul class="links"&gt;_x000D_
+                                                                &lt;li&gt;&lt;a href="#"&gt;iPhone X&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                                &lt;li&gt;&lt;a href="#"&gt;iPhone XR&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                            &lt;/ul&gt;_x000D_
+                                                        &lt;/div&gt;_x000D_
+                                                        _x000D_
+_x000D_
+                                                        &lt;div class="col-xs-12 col-sm-6 col-md-4 col-menu banner-image"&gt;_x000D_
+                                                            &lt;img class="img-responsive"_x000D_
+                                                                src="assets\images\banners\top-menu-banner.jpg"_x000D_
+                                                                alt=""&gt;_x000D_
+                                                        &lt;/div&gt;_x000D_
+                                                        _x000D_
+                                                    &lt;/div&gt;_x000D_
+                                                &lt;/div&gt;_x000D_
+                                            &lt;/li&gt;_x000D_
+                                        &lt;/ul&gt;_x000D_
+                                    &lt;/li&gt;_x000D_
+                                    &lt;li class="dropdown mega-menu"&gt;_x000D_
+                                        &lt;a href="category.html" data-hover="dropdown" class="dropdown-toggle"_x000D_
+                                            data-toggle="dropdown"&gt;iPad &lt;span_x000D_
+                                                class="menu-label hot-menu hidden-xs"&gt;hot&lt;/span&gt; &lt;/a&gt;_x000D_
+                                        &lt;ul class="dropdown-menu container"&gt;_x000D_
+                                            &lt;li&gt;_x000D_
+                                                &lt;div class="yamm-content"&gt;_x000D_
+                                                    &lt;div class="row"&gt;_x000D_
+                                                        &lt;div class="col-xs-12 col-sm-12 col-md-2 col-menu"&gt;_x000D_
+                                                            &lt;h2 class="title"&gt;iPad Mini&lt;/h2&gt;_x000D_
+                                                            &lt;ul class="links"&gt;_x000D_
+                                                                &lt;li&gt;&lt;a href="#"&gt;iPad Mini 2 Wifi 4G&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                            &lt;/ul&gt;_x000D_
+                                                        &lt;/div&gt;_x000D_
+                                                        _x000D_
+_x000D_
+                                                        &lt;div class="col-xs-12 col-sm-12 col-md-2 col-menu"&gt;_x000D_
+                                                            &lt;h2 class="title"&gt;iPad Air&lt;/h2&gt;_x000D_
+                                                            &lt;ul class="links"&gt;_x000D_
+                                                                &lt;li&gt;&lt;a href="#"&gt;iPad Air Wifi 4G&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                                &lt;li&gt;&lt;a href="#"&gt;iPad Air 2 Wifi 4G&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                            &lt;/ul&gt;_x000D_
+                                                        &lt;/div&gt;_x000D_
+                                                        _x000D_
+_x000D_
+                                                        &lt;div_x000D_
+                                                            class="col-xs-12 col-sm-12 col-md-4 col-menu custom-banner"&gt;_x000D_
+                                                            &lt;a href="#"&gt;&lt;img alt=""_x000D_
+                                                                    src="assets\images\banners\banner-side.png"&gt;&lt;/a&gt;_x000D_
+                                                        &lt;/div&gt;_x000D_
+                                                    &lt;/div&gt;_x000D_
+                                                    _x000D_
+                                                &lt;/div&gt;_x000D_
+                                                _x000D_
+                                            &lt;/li&gt;_x000D_
+                                        &lt;/ul&gt;_x000D_
+                                    &lt;/li&gt;_x000D_
+                                    &lt;li class="dropdown hidden-sm"&gt; &lt;a href="category.html"&gt;Apple Watch&lt;/a&gt; &lt;/li&gt;_x000D_
+                                    &lt;li class="dropdown"&gt; &lt;a href="contact.html"&gt;SamSung &lt;span_x000D_
+                                                class="menu-label hot-menu hidden-xs"&gt;hot&lt;/span&gt; &lt;/a&gt; &lt;/li&gt;_x000D_
+                                    &lt;li class="dropdown"&gt; &lt;a href="contact.html"&gt;Oppo&lt;/a&gt; &lt;/li&gt;_x000D_
+                                    &lt;li class="dropdown"&gt; &lt;a href="contact.html"&gt;Xiaomi&lt;/a&gt; &lt;/li&gt;_x000D_
+                                    &lt;li class="dropdown"&gt; &lt;a href="contact.html"&gt;Vivo&lt;/a&gt; &lt;/li&gt;_x000D_
+                                    &lt;li class="dropdown"&gt; &lt;a href="contact.html"&gt;Realme&lt;/a&gt; &lt;/li&gt;_x000D_
+                                    &lt;li class="dropdown"&gt; &lt;a href="contact.html"&gt;Phá»¥ kiá»‡n&lt;/a&gt; &lt;/li&gt;_x000D_
+                                    &lt;li class="dropdown"&gt; &lt;a href="#" class="dropdown-toggle"_x000D_
+                                            data-hover="dropdown" data-toggle="dropdown"&gt;Pages&lt;/a&gt;_x000D_
+                                        &lt;ul class="dropdown-menu pages"&gt;_x000D_
+                                            &lt;li&gt;_x000D_
+                                                &lt;div class="yamm-content"&gt;_x000D_
+                                                    &lt;div class="row"&gt;_x000D_
+                                                        &lt;div class="col-xs-12 col-menu"&gt;_x000D_
+                                                            &lt;ul class="links"&gt;_x000D_
+                                                                &lt;li&gt;&lt;a href="home.html"&gt;Home&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                                &lt;li&gt;&lt;a href="category.html"&gt;Category&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                                &lt;li&gt;&lt;a href="detail.html"&gt;Detail&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                                &lt;li&gt;&lt;a href="shopping-cart.html"&gt;Shopping Cart_x000D_
+                                                                        Summary&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                                &lt;li&gt;&lt;a href="checkout.html"&gt;Checkout&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                                &lt;li&gt;&lt;a href="blog.html"&gt;Blog&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                                &lt;li&gt;&lt;a href="blog-details.html"&gt;Blog Detail&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                                &lt;li&gt;&lt;a href="contact.html"&gt;Contact&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                                &lt;li&gt;&lt;a href="sign-in.html"&gt;Sign In&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                                &lt;li&gt;&lt;a href="my-wishlist.html"&gt;Wishlist&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                                &lt;li&gt;&lt;a href="terms-conditions.html"&gt;Terms and_x000D_
+                                                                        Condition&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                                &lt;li&gt;&lt;a href="track-orders.html"&gt;Track Orders&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                                &lt;li&gt;&lt;a_x000D_
+                                                                        href="product-comparison.html"&gt;Product-Comparison&lt;/a&gt;_x000D_
+                                                                &lt;/li&gt;_x000D_
+                                                                &lt;li&gt;&lt;a href="faq.html"&gt;FAQ&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                                &lt;li&gt;&lt;a href="404.html"&gt;404&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                            &lt;/ul&gt;_x000D_
+                                                        &lt;/div&gt;_x000D_
+                                                    &lt;/div&gt;_x000D_
+                                                &lt;/div&gt;_x000D_
+                                            &lt;/li&gt;_x000D_
+                                        &lt;/ul&gt;_x000D_
+                                    &lt;/li&gt;_x000D_
+                                    &lt;li class="dropdown  navbar-right special-menu"&gt; &lt;a href="#"&gt;Todays_x000D_
+                                            offer&lt;/a&gt; &lt;/li&gt;_x000D_
+                                &lt;/ul&gt;_x000D_
+                                _x000D_
+                                &lt;div class="clearfix"&gt;&lt;/div&gt;_x000D_
+                            &lt;/div&gt;_x000D_
+                            _x000D_
+                        &lt;/div&gt;_x000D_
+                        _x000D_
+_x000D_
+                    &lt;/div&gt;_x000D_
+                    _x000D_
+                &lt;/div&gt;_x000D_
+                _x000D_
+            &lt;/div&gt;_x000D_
+            _x000D_
+_x000D_
+        &lt;/div&gt;_x000D_
+        _x000D_
+        _x000D_
+_x000D_
+    &lt;/header&gt;_x000D_
+    &lt;div class="share-fast-mall"&gt;_x000D_
+        &lt;div class="youtube-button"&gt;_x000D_
+            &lt;a href="https://www.youtube.com/channel/your-channel-id-here" target="_blank" title="link youtube"&gt;&lt;i_x000D_
+                    class="fa-brands fa-youtube"&gt;&lt;/i&gt;&lt;/a&gt;_x000D_
+        &lt;/div&gt;_x000D_
+        &lt;div class="fb-button"&gt;_x000D_
+            &lt;a href="https://www.youtube.com/channel/your-channel-id-here" target="_blank" title="link facebook"&gt;&lt;i_x000D_
+                    class="fa-brands fa-facebook-f"&gt;&lt;/i&gt;&lt;/a&gt;_x000D_
+        &lt;/div&gt;_x000D_
+        &lt;div class="tt-button"&gt;_x000D_
+            &lt;a href="https://www.youtube.com/channel/your-channel-id-here" target="_blank" title="link tiktok"&gt;&lt;i_x000D_
+                    class="fa-brands fa-tiktok"&gt;&lt;/i&gt;&lt;/a&gt;_x000D_
+        &lt;/div&gt;_x000D_
+    &lt;/div&gt;_x000D_
+_x000D_
+    &lt;div class="body-content outer-top-xs" id="top-banner-and-menu"&gt;_x000D_
+        &lt;div class="container"&gt;_x000D_
+            &lt;div class="row"&gt;_x000D_
+                &lt;div class="col-xs-12 col-sm-12 col-md-3 sidebar"&gt;_x000D_
+                    &lt;div class="side-menu animate-dropdown outer-bottom-xs"&gt;_x000D_
+                        &lt;div class="head"&gt;&lt;i class="icon fa fa-align-justify fa-fw"&gt;&lt;/i&gt; Danh má»¥c sáº£n pháº©m&lt;/div&gt;_x000D_
+                        &lt;nav class="yamm megamenu-horizontal"&gt;_x000D_
+                            &lt;ul class="nav"&gt;_x000D_
+                                &lt;li class="dropdown menu-item"&gt; &lt;a href="#" class="dropdown-toggle"_x000D_
+                                        data-toggle="dropdown"&gt;&lt;i class="icon fa-solid fa-mobile-screen-button"_x000D_
+                                            style="color: #000000;" aria-hidden="true"&gt;&lt;/i&gt;iPhone&lt;/a&gt;_x000D_
+                                    &lt;ul class="dropdown-menu mega-menu"&gt;_x000D_
+                                        &lt;li&gt;_x000D_
+                                            &lt;div class="yamm-content "&gt;_x000D_
+                                                &lt;div class="row"&gt;_x000D_
+                                                    &lt;div class="col-xs-12 col-sm-6 col-md-2 col-menu"&gt;_x000D_
+                                                        &lt;h2 class="title"&gt;iPhone 14 Series&lt;/h2&gt;_x000D_
+                                                        &lt;ul class="links"&gt;_x000D_
+                                                            &lt;li&gt;&lt;a href="#"&gt;iPhone 14 Pro Max&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                            &lt;li&gt;&lt;a href="#"&gt;iPhone 14 Pro&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                            &lt;li&gt;&lt;a href="#"&gt;iPhone 14 Plus&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                            &lt;li&gt;&lt;a href="#"&gt;iPhone 14&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                        &lt;/ul&gt;_x000D_
+                                                    &lt;/div&gt;_x000D_
+_x000D_
+                                                    &lt;div class="col-xs-12 col-sm-6 col-md-2 col-menu"&gt;_x000D_
+                                                        &lt;h2 class="title"&gt;iPhone 13 Series&lt;/h2&gt;_x000D_
+                                                        &lt;ul class="links"&gt;_x000D_
+                                                            &lt;li&gt;&lt;a href="#"&gt;iPhone 13 Mini&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                            &lt;li&gt;&lt;a href="#"&gt;iPhone 13&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                            &lt;li&gt;&lt;a href="#"&gt;iPhone 13 Pro &lt;/a&gt;&lt;/li&gt;_x000D_
+                                                            &lt;li&gt;&lt;a href="#"&gt;iPhone 13 Pro Max&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                        &lt;/ul&gt;_x000D_
+                                                    &lt;/div&gt;_x000D_
+_x000D_
+                                                    &lt;div class="col-xs-12 col-sm-6 col-md-2 col-menu"&gt;_x000D_
+                                                        &lt;h2 class="title"&gt;iPhone 12 Series&lt;/h2&gt;_x000D_
+                                                        &lt;ul class="links"&gt;_x000D_
+                                                            &lt;li&gt;&lt;a href="#"&gt;iPhone 12&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                        &lt;/ul&gt;_x000D_
+                                                    &lt;/div&gt;_x000D_
+_x000D_
+                                                    &lt;div class="col-xs-12 col-sm-6 col-md-2 col-menu"&gt;_x000D_
+                                                        &lt;h2 class="title"&gt;iPhone 11 Series&lt;/h2&gt;_x000D_
+                                                        &lt;ul class="links"&gt;_x000D_
+                                                            &lt;li&gt;&lt;a href="#"&gt;iPhone 11&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                            &lt;li&gt;&lt;a href="#"&gt;iPhone 11 Pro&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                            &lt;li&gt;&lt;a href="#"&gt;iPhone 11 Pro Max&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                        &lt;/ul&gt;_x000D_
+                                                    &lt;/div&gt;_x000D_
+                                                    _x000D_
+                                                    &lt;div class="col-xs-12 col-sm-6 col-md-2 col-menu"&gt;_x000D_
+                                                        &lt;h2 class="title"&gt;iPhone XS / iPhone XS Max&lt;/h2&gt;_x000D_
+                                                        &lt;ul class="links"&gt;_x000D_
+                                                            &lt;li&gt;&lt;a href="#"&gt;iPhone XS&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                            &lt;li&gt;&lt;a href="#"&gt;iPhone XS Max&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                        &lt;/ul&gt;_x000D_
+                                                    &lt;/div&gt;_x000D_
+                                                    _x000D_
+                                                    &lt;div class="col-xs-12 col-sm-6 col-md-2 col-menu"&gt;_x000D_
+                                                        &lt;h2 class="title"&gt;iPhone X / iPhone XR&lt;/h2&gt;_x000D_
+                                                        &lt;ul class="links"&gt;_x000D_
+                                                            &lt;li&gt;&lt;a href="#"&gt;iPhone X&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                            &lt;li&gt;&lt;a href="#"&gt;iPhone XR&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                        &lt;/ul&gt;_x000D_
+                                                    &lt;/div&gt;_x000D_
+_x000D_
+                                                    &lt;div class="col-xs-12 col-sm-6 col-md-4 col-menu banner-image"&gt;_x000D_
+                                                        &lt;img class="img-responsive"_x000D_
+                                                            src="assets\images\banners\top-menu-banner.jpg"_x000D_
+                                                            alt=""&gt;_x000D_
+                                                    &lt;/div&gt;_x000D_
+                                                &lt;/div&gt;_x000D_
+                                            &lt;/div&gt;_x000D_
+                                        &lt;/li&gt;_x000D_
+                                    &lt;/ul&gt;_x000D_
+                                &lt;/li&gt;_x000D_
+_x000D_
+                                &lt;li class="dropdown menu-item"&gt; &lt;a href="#" class="dropdown-toggle"_x000D_
+                                        data-toggle="dropdown"&gt;&lt;i class="icon fa-solid fa-tablet-screen-button"_x000D_
+                                            style="color: #000000;" aria-hidden="true"&gt;&lt;/i&gt;iPad&lt;/a&gt;_x000D_
+                                    _x000D_
+                                    &lt;ul class="dropdown-menu mega-menu"&gt;_x000D_
+                                        &lt;li class="yamm-content"&gt;_x000D_
+                                            &lt;div class="row"&gt;_x000D_
+                                                &lt;div class="col-xs-12 col-sm-12 col-lg-4"&gt;_x000D_
+                                                    &lt;ul&gt;_x000D_
+                                                        &lt;li&gt;&lt;a href="#"&gt;Gaming&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                        &lt;li&gt;&lt;a href="#"&gt;Laptop Skins&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                        &lt;li&gt;&lt;a href="#"&gt;Apple&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                        &lt;li&gt;&lt;a href="#"&gt;Dell&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                        &lt;li&gt;&lt;a href="#"&gt;Lenovo&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                        &lt;li&gt;&lt;a href="#"&gt;Microsoft&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                        &lt;li&gt;&lt;a href="#"&gt;Asus&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                        &lt;li&gt;&lt;a href="#"&gt;Adapters&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                        &lt;li&gt;&lt;a href="#"&gt;Batteries&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                        &lt;li&gt;&lt;a href="#"&gt;Cooling Pads&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                    &lt;/ul&gt;_x000D_
+                                                &lt;/div&gt;_x000D_
+                                                &lt;div class="col-xs-12 col-sm-12 col-lg-4"&gt;_x000D_
+                                                    &lt;ul&gt;_x000D_
+                                                        &lt;li&gt;&lt;a href="#"&gt;Routers &amp;amp; Modems&lt;/a&gt;&lt;/li&gt;_x000D_
+                                                        &lt;li&gt;&lt;a href="#"&gt;CPUs, Proc</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="167" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="171" formatCode="[$-1010000]d/m/yyyy;@"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +584,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -45,12 +616,89 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +978,128 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:AT3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.44140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="19.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="2"/>
+    <col min="4" max="4" width="24.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="19.21875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" style="2" customWidth="1"/>
+    <col min="9" max="12" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:46" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="8"/>
+    </row>
+    <row r="2" spans="1:46" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="4">
+        <v>45874</v>
+      </c>
+      <c r="E2" s="4">
+        <v>45875</v>
+      </c>
+      <c r="F2" s="4">
+        <v>45876</v>
+      </c>
+      <c r="G2" s="4">
+        <v>45877</v>
+      </c>
+      <c r="H2" s="4">
+        <v>45878</v>
+      </c>
+      <c r="I2" s="4">
+        <v>45879</v>
+      </c>
+      <c r="J2" s="4">
+        <v>45880</v>
+      </c>
+      <c r="K2" s="4">
+        <v>45881</v>
+      </c>
+      <c r="L2" s="4">
+        <v>45882</v>
+      </c>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="4"/>
+      <c r="AE2" s="4"/>
+      <c r="AF2" s="4"/>
+      <c r="AG2" s="4"/>
+      <c r="AH2" s="4"/>
+      <c r="AI2" s="4"/>
+      <c r="AJ2" s="4"/>
+      <c r="AK2" s="4"/>
+      <c r="AL2" s="4"/>
+      <c r="AM2" s="4"/>
+      <c r="AN2" s="4"/>
+      <c r="AO2" s="4"/>
+      <c r="AP2" s="4"/>
+      <c r="AQ2" s="4"/>
+      <c r="AR2" s="4"/>
+      <c r="AS2" s="4"/>
+      <c r="AT2" s="5"/>
+    </row>
+    <row r="3" spans="1:46" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:L1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>